<commit_message>
suppression des onglets unitils (emploi, evenement ..)
</commit_message>
<xml_diff>
--- a/Excels_for_bg5/Liste_des_étudiants_d_ L3_2023-2024.xlsx
+++ b/Excels_for_bg5/Liste_des_étudiants_d_ L3_2023-2024.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medto\Desktop\Docs\Xcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamano.7\Desktop\CI\CI\Excels_for_bg5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CEF6D4-469D-4B63-983B-4E1AB44B0957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -300,9 +299,6 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>departemen</t>
-  </si>
-  <si>
     <t>licence</t>
   </si>
   <si>
@@ -322,12 +318,15 @@
   </si>
   <si>
     <t>is_chef_departement</t>
+  </si>
+  <si>
+    <t>departement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -719,11 +718,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -747,28 +746,28 @@
         <v>82</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="L1" s="6"/>
     </row>
@@ -786,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="6">
         <v>0</v>
@@ -824,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="6">
         <v>0</v>
@@ -862,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="6">
         <v>0</v>
@@ -900,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
@@ -938,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
@@ -976,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
@@ -1014,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -1052,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="6">
         <v>0</v>
@@ -1090,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -1128,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="6">
         <v>0</v>
@@ -1166,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
@@ -1204,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F13" s="6">
         <v>0</v>
@@ -1242,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
@@ -1280,7 +1279,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F15" s="6">
         <v>0</v>
@@ -1318,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="6">
         <v>0</v>
@@ -1356,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F17" s="6">
         <v>0</v>
@@ -1394,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
@@ -1432,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F19" s="6">
         <v>0</v>
@@ -1470,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F20" s="6">
         <v>0</v>
@@ -1508,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
@@ -1546,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F22" s="6">
         <v>0</v>
@@ -1584,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F23" s="6">
         <v>0</v>
@@ -1622,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F24" s="6">
         <v>0</v>
@@ -1660,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F25" s="6">
         <v>0</v>
@@ -1698,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F26" s="6">
         <v>0</v>
@@ -1736,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F27" s="6">
         <v>0</v>
@@ -1774,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F28" s="6">
         <v>0</v>
@@ -1812,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F29" s="6">
         <v>0</v>
@@ -1850,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F30" s="6">
         <v>0</v>
@@ -1888,7 +1887,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F31" s="6">
         <v>0</v>
@@ -1926,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F32" s="6">
         <v>0</v>
@@ -1964,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F33" s="6">
         <v>0</v>
@@ -2002,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F34" s="6">
         <v>0</v>
@@ -2040,7 +2039,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F35" s="6">
         <v>0</v>
@@ -2078,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F36" s="6">
         <v>0</v>
@@ -2116,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F37" s="6">
         <v>0</v>
@@ -2154,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F38" s="6">
         <v>0</v>
@@ -2192,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F39" s="6">
         <v>0</v>
@@ -2230,7 +2229,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F40" s="6">
         <v>0</v>
@@ -2268,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F41" s="6">
         <v>0</v>
@@ -2306,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F42" s="6">
         <v>0</v>
@@ -2344,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F43" s="6">
         <v>0</v>
@@ -2382,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F44" s="6">
         <v>0</v>
@@ -2420,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F45" s="6">
         <v>0</v>
@@ -2458,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F46" s="6">
         <v>0</v>
@@ -2496,7 +2495,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F47" s="6">
         <v>0</v>
@@ -2534,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F48" s="6">
         <v>0</v>
@@ -2572,7 +2571,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F49" s="6">
         <v>0</v>
@@ -2610,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F50" s="6">
         <v>0</v>
@@ -2648,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F51" s="6">
         <v>0</v>
@@ -2686,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F52" s="6">
         <v>0</v>
@@ -2724,7 +2723,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F53" s="6">
         <v>0</v>
@@ -2762,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F54" s="6">
         <v>0</v>
@@ -2800,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F55" s="6">
         <v>0</v>
@@ -2838,7 +2837,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F56" s="6">
         <v>0</v>
@@ -2876,7 +2875,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F57" s="6">
         <v>0</v>

</xml_diff>